<commit_message>
names changed for prokerala
</commit_message>
<xml_diff>
--- a/data/naksatras.xlsx
+++ b/data/naksatras.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="210">
   <si>
     <t xml:space="preserve">Marriage Compatibility Chart</t>
   </si>
@@ -514,6 +514,9 @@
     <t xml:space="preserve">Krittika</t>
   </si>
   <si>
+    <t xml:space="preserve">Krithika</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rohini</t>
   </si>
   <si>
@@ -613,7 +616,7 @@
     <t xml:space="preserve">Utthiradam</t>
   </si>
   <si>
-    <t xml:space="preserve">Uttara Ashada</t>
+    <t xml:space="preserve">Uttara Ashadha</t>
   </si>
   <si>
     <t xml:space="preserve">Thiruvonam</t>
@@ -625,7 +628,7 @@
     <t xml:space="preserve">Avittam</t>
   </si>
   <si>
-    <t xml:space="preserve">Dhanistha</t>
+    <t xml:space="preserve">Dhanishta</t>
   </si>
   <si>
     <t xml:space="preserve">Sathayam</t>
@@ -965,7 +968,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1056,9 +1059,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>227880</xdr:colOff>
+      <xdr:colOff>227520</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>408960</xdr:rowOff>
+      <xdr:rowOff>408600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1068,7 +1071,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="374040" y="1095480"/>
-          <a:ext cx="123120" cy="551880"/>
+          <a:ext cx="122760" cy="551520"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
           <a:avLst>
@@ -1118,9 +1121,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1047240</xdr:colOff>
+      <xdr:colOff>1046880</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>570600</xdr:rowOff>
+      <xdr:rowOff>570240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1130,7 +1133,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1260000" y="1657440"/>
-          <a:ext cx="494640" cy="151560"/>
+          <a:ext cx="494280" cy="151200"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -1185,9 +1188,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>227880</xdr:colOff>
+      <xdr:colOff>227520</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1197,7 +1200,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="374040" y="1095480"/>
-          <a:ext cx="123120" cy="551880"/>
+          <a:ext cx="122760" cy="551520"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
           <a:avLst>
@@ -1247,9 +1250,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>504000</xdr:colOff>
+      <xdr:colOff>503640</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>199080</xdr:rowOff>
+      <xdr:rowOff>198720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1259,7 +1262,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="534960" y="1276200"/>
-          <a:ext cx="676440" cy="161280"/>
+          <a:ext cx="676080" cy="160920"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -1311,7 +1314,7 @@
   <dimension ref="A1:AM44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="A2 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.11328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5810,10 +5813,10 @@
   <dimension ref="A1:DG116"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2030" ySplit="1875" topLeftCell="A97" activePane="bottomLeft" state="split"/>
+      <pane xSplit="1899" ySplit="1875" topLeftCell="A97" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
       <selection pane="topRight" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="B7" activeCellId="1" sqref="A2 B7"/>
       <selection pane="bottomRight" activeCell="A97" activeCellId="0" sqref="A97"/>
     </sheetView>
   </sheetViews>
@@ -42422,7 +42425,7 @@
   <dimension ref="A1:DE109"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="1" sqref="A2 I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.11328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -78314,12 +78317,12 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.74609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="30" width="17.56"/>
   </cols>
   <sheetData>
     <row r="1" s="37" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -78329,13 +78332,13 @@
       <c r="B1" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="I1" s="0"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="30" t="s">
         <v>160</v>
       </c>
     </row>
@@ -78343,7 +78346,7 @@
       <c r="A3" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="30" t="s">
         <v>161</v>
       </c>
     </row>
@@ -78351,205 +78354,205 @@
       <c r="A4" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>162</v>
+      <c r="B4" s="30" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="B6" s="0" t="s">
         <v>165</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="B7" s="0" t="s">
         <v>167</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="B8" s="0" t="s">
         <v>169</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="B9" s="0" t="s">
         <v>171</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="B10" s="0" t="s">
         <v>173</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="B11" s="0" t="s">
         <v>175</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="B12" s="0" t="s">
         <v>177</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="B13" s="0" t="s">
         <v>179</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="B14" s="0" t="s">
         <v>181</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="B15" s="0" t="s">
         <v>183</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="B17" s="0" t="s">
         <v>186</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="B18" s="0" t="s">
         <v>188</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="B19" s="0" t="s">
         <v>190</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="B20" s="0" t="s">
         <v>192</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="B21" s="0" t="s">
         <v>194</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="B22" s="0" t="s">
         <v>196</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="B23" s="0" t="s">
         <v>198</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="B24" s="0" t="s">
         <v>200</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="B25" s="0" t="s">
         <v>202</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="B26" s="0" t="s">
         <v>204</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="B27" s="0" t="s">
         <v>206</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>208</v>
+      <c r="A30" s="30" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>